<commit_message>
updated framework suggestions and review tracker
</commit_message>
<xml_diff>
--- a/Documents/FrameworkSuggestions.xlsx
+++ b/Documents/FrameworkSuggestions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbolak01c\Desktop\Documents\BSA Projects\Century\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Century\Century_old_testng\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>Enable Fallback mechanism for object verification failures. Try out different approach at runtime to resolve the issue</t>
   </si>
@@ -242,6 +242,18 @@
   </si>
   <si>
     <t>Multi-Dependency</t>
+  </si>
+  <si>
+    <t>DSL/Keyword based development</t>
+  </si>
+  <si>
+    <t>Harsh/Team?</t>
+  </si>
+  <si>
+    <t>Set up a high level framework for functional testers to develop scripts with ease</t>
+  </si>
+  <si>
+    <t>https://github.comcast.com/quality-driven-delivery/BSA_Selenium_Core</t>
   </si>
 </sst>
 </file>
@@ -318,11 +330,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -331,9 +340,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -650,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,849 +674,868 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
         <v>4</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>42591</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>42591</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>42612</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>42591</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>2</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>42591</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
         <v>2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>42591</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>42591</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>42591</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>42629</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>2</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>42591</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
         <v>3</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>42591</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
         <v>2</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>42591</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>42591</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>42591</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="E14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>42606</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G15" s="4">
         <v>42591</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" s="4">
+        <v>42606</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="5">
-        <v>42591</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="G17" s="4">
+        <v>42606</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>42606</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4">
+        <v>42606</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2</v>
+      </c>
+      <c r="G20" s="4">
+        <v>42606</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="E21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="2">
+        <v>3</v>
+      </c>
+      <c r="G21" s="4">
+        <v>42606</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>42606</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4">
+        <v>42611</v>
+      </c>
+      <c r="H23" s="4">
+        <v>42619</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4">
+        <v>42626</v>
+      </c>
+      <c r="H24" s="4">
+        <v>42629</v>
+      </c>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="G14" s="5">
-        <v>42606</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="G25" s="4">
+        <v>42632</v>
+      </c>
+      <c r="H25" s="4">
+        <v>42642</v>
+      </c>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>42591</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3">
-        <v>3</v>
-      </c>
-      <c r="G16" s="5">
-        <v>42606</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5">
-        <v>42606</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="5">
-        <v>42606</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3">
-        <v>2</v>
-      </c>
-      <c r="G19" s="5">
-        <v>42606</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="3">
-        <v>2</v>
-      </c>
-      <c r="G20" s="5">
-        <v>42606</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="3">
-        <v>3</v>
-      </c>
-      <c r="G21" s="5">
-        <v>42606</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3">
+      <c r="E26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="2">
         <v>4</v>
       </c>
-      <c r="G22" s="5">
-        <v>42606</v>
-      </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5">
-        <v>42611</v>
-      </c>
-      <c r="H23" s="5">
-        <v>42619</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="5">
-        <v>42626</v>
-      </c>
-      <c r="H24" s="5">
-        <v>42629</v>
-      </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="3">
-        <v>2</v>
-      </c>
-      <c r="G25" s="5">
-        <v>42632</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="G26" s="4">
+        <v>42643</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G27" s="2"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G28" s="2"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G29" s="2"/>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="2"/>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G31" s="2"/>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G32" s="2"/>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="2"/>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="2"/>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="2"/>
+      <c r="G35" s="1"/>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G36" s="2"/>
+      <c r="G36" s="1"/>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="2"/>
+      <c r="G37" s="1"/>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="2"/>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="2"/>
+      <c r="G39" s="1"/>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G40" s="2"/>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G41" s="2"/>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G42" s="2"/>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G43" s="2"/>
+      <c r="G43" s="1"/>
     </row>
     <row r="44" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G44" s="2"/>
+      <c r="G44" s="1"/>
     </row>
     <row r="45" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G45" s="2"/>
+      <c r="G45" s="1"/>
     </row>
     <row r="46" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G46" s="2"/>
+      <c r="G46" s="1"/>
     </row>
     <row r="47" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G47" s="2"/>
+      <c r="G47" s="1"/>
     </row>
     <row r="48" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G48" s="2"/>
+      <c r="G48" s="1"/>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49" s="2"/>
+      <c r="G49" s="1"/>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G50" s="2"/>
+      <c r="G50" s="1"/>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G51" s="2"/>
+      <c r="G51" s="1"/>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G52" s="2"/>
+      <c r="G52" s="1"/>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G53" s="2"/>
+      <c r="G53" s="1"/>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54" s="2"/>
+      <c r="G54" s="1"/>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G55" s="2"/>
+      <c r="G55" s="1"/>
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G56" s="2"/>
+      <c r="G56" s="1"/>
     </row>
     <row r="57" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G57" s="2"/>
+      <c r="G57" s="1"/>
     </row>
     <row r="58" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G58" s="2"/>
+      <c r="G58" s="1"/>
     </row>
     <row r="59" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G59" s="2"/>
+      <c r="G59" s="1"/>
     </row>
     <row r="60" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G60" s="2"/>
+      <c r="G60" s="1"/>
     </row>
     <row r="61" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G61" s="2"/>
+      <c r="G61" s="1"/>
     </row>
     <row r="62" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G62" s="2"/>
+      <c r="G62" s="1"/>
     </row>
     <row r="63" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G63" s="2"/>
+      <c r="G63" s="1"/>
     </row>
     <row r="64" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G64" s="2"/>
+      <c r="G64" s="1"/>
     </row>
     <row r="65" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G65" s="2"/>
+      <c r="G65" s="1"/>
     </row>
     <row r="66" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G66" s="2"/>
+      <c r="G66" s="1"/>
     </row>
     <row r="67" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G67" s="2"/>
+      <c r="G67" s="1"/>
     </row>
     <row r="68" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G68" s="2"/>
+      <c r="G68" s="1"/>
     </row>
     <row r="69" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G69" s="2"/>
+      <c r="G69" s="1"/>
     </row>
     <row r="70" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G70" s="2"/>
+      <c r="G70" s="1"/>
     </row>
     <row r="71" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G71" s="2"/>
+      <c r="G71" s="1"/>
     </row>
     <row r="72" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G72" s="2"/>
+      <c r="G72" s="1"/>
     </row>
     <row r="73" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G73" s="2"/>
+      <c r="G73" s="1"/>
     </row>
     <row r="74" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G74" s="2"/>
+      <c r="G74" s="1"/>
     </row>
     <row r="75" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G75" s="2"/>
+      <c r="G75" s="1"/>
     </row>
     <row r="76" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G76" s="2"/>
+      <c r="G76" s="1"/>
     </row>
     <row r="77" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G77" s="2"/>
+      <c r="G77" s="1"/>
     </row>
     <row r="78" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G78" s="2"/>
+      <c r="G78" s="1"/>
     </row>
     <row r="79" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G79" s="2"/>
+      <c r="G79" s="1"/>
     </row>
     <row r="80" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G80" s="2"/>
+      <c r="G80" s="1"/>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G81" s="2"/>
+      <c r="G81" s="1"/>
     </row>
     <row r="82" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G82" s="2"/>
+      <c r="G82" s="1"/>
     </row>
     <row r="83" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G83" s="2"/>
+      <c r="G83" s="1"/>
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G84" s="2"/>
+      <c r="G84" s="1"/>
     </row>
     <row r="85" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G85" s="2"/>
+      <c r="G85" s="1"/>
     </row>
     <row r="86" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G86" s="2"/>
+      <c r="G86" s="1"/>
     </row>
     <row r="87" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G87" s="2"/>
+      <c r="G87" s="1"/>
     </row>
     <row r="88" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G88" s="2"/>
+      <c r="G88" s="1"/>
     </row>
     <row r="89" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G89" s="2"/>
+      <c r="G89" s="1"/>
     </row>
     <row r="90" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G90" s="2"/>
+      <c r="G90" s="1"/>
     </row>
     <row r="91" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G91" s="2"/>
+      <c r="G91" s="1"/>
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G92" s="2"/>
+      <c r="G92" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I25"/>
   <hyperlinks>
     <hyperlink ref="I8" r:id="rId1"/>
+    <hyperlink ref="I26" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added few more review comments
</commit_message>
<xml_diff>
--- a/Documents/FrameworkSuggestions.xlsx
+++ b/Documents/FrameworkSuggestions.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$26</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -330,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -345,6 +345,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -656,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1278,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1302,9 +1303,11 @@
       <c r="H25" s="4">
         <v>42642</v>
       </c>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I25" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1327,9 +1330,7 @@
         <v>42643</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G27" s="1"/>
@@ -1530,10 +1531,10 @@
       <c r="G92" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I25"/>
+  <autoFilter ref="A1:I26"/>
   <hyperlinks>
     <hyperlink ref="I8" r:id="rId1"/>
-    <hyperlink ref="I26" r:id="rId2"/>
+    <hyperlink ref="I25" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>

</xml_diff>